<commit_message>
Add: Group10 test in different xlsx sheet
</commit_message>
<xml_diff>
--- a/FinalRequirements .xlsx
+++ b/FinalRequirements .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritazyaupreti/Desktop/UNIVERSITY/4th Sem/Fundamentals of Software Engineering/Project/cse3310-sp25-003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2F51A4-6F4A-3C4C-A650-DE335FDA7F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0611AAAF-FEBE-4243-9C75-80F90DE58563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3100" windowWidth="37260" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31360" yWindow="-3100" windowWidth="37260" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="871">
   <si>
     <t>Testing</t>
   </si>
@@ -2839,6 +2839,9 @@
   </si>
   <si>
     <t>removed msg() and used socket.send() instead</t>
+  </si>
+  <si>
+    <t>TEST Prodecure and Defect Identification is in different spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -4503,7 +4506,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>3915720</xdr:colOff>
       <xdr:row>149</xdr:row>
-      <xdr:rowOff>804767</xdr:rowOff>
+      <xdr:rowOff>804766</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4761,7 +4764,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>9530280</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>2053</xdr:rowOff>
+      <xdr:rowOff>2054</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5776,8 +5779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="47"/>
@@ -5880,7 +5883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="144">
+    <row r="4" spans="1:20" ht="240">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -5899,7 +5902,9 @@
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="43"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>870</v>
+      </c>
       <c r="I4" s="44" t="s">
         <v>22</v>
       </c>

</xml_diff>